<commit_message>
limit up analyze update
</commit_message>
<xml_diff>
--- a/excel/limit_up_history.xlsx
+++ b/excel/limit_up_history.xlsx
@@ -29,12 +29,24 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F2F2F2"/>
+        <bgColor rgb="00F2F2F2"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +67,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,6 +446,17 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -481,1796 +506,1796 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>2025-04-14</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>1进2</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>6.33%</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>30.38%</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>63.29%</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="2" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>2025-04-14</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>2进3</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>28.57%</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>28.57%</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>42.86%</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="2" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>2025-04-14</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>3进4</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>25.00%</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>25.00%</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="G4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>2025-04-14</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>5进6</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
+      <c r="G5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>2025-04-14</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>7进8</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
+      <c r="G6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>2025-04-15</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>1进2</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>19.57%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>30.43%</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="3" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>2025-04-15</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>2进3</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>60.00%</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
         <is>
           <t>40.00%</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
+      <c r="H8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>2025-04-15</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>3进4</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>40.00%</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="3" t="inlineStr">
         <is>
           <t>20.00%</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr">
         <is>
           <t>40.00%</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>2025-04-15</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>4进5</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="3" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" t="n">
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>2025-04-16</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>1进2</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>29.17%</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>37.50%</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="G11" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" s="2" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>2025-04-16</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>2进3</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>72.73%</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>9.09%</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>18.18%</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="G12" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="H12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>2025-04-16</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>3进4</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>66.67%</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>2025-04-16</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>4进5</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t>66.67%</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
+      <c r="G14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>2025-04-16</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>5进6</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" t="n">
+      <c r="G15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>2025-04-16</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
+      <c r="B16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>7进8</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
+      <c r="G16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>2025-04-16</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
+      <c r="B17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>8进9</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" t="n">
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="3" t="inlineStr">
         <is>
           <t>2025-04-17</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>1进2</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" s="3" t="inlineStr">
         <is>
           <t>15.52%</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E18" s="3" t="inlineStr">
         <is>
           <t>18.97%</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>65.52%</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" s="3" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>2025-04-17</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>2进3</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" s="3" t="inlineStr">
         <is>
           <t>22.22%</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" s="3" t="inlineStr">
         <is>
           <t>11.11%</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
         <is>
           <t>66.67%</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H19" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" t="n">
+      <c r="H19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="3" t="inlineStr">
         <is>
           <t>2025-04-17</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="3" t="inlineStr">
         <is>
           <t>3进4</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" s="3" t="inlineStr">
         <is>
           <t>40.00%</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E20" s="3" t="inlineStr">
         <is>
           <t>30.00%</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="3" t="inlineStr">
         <is>
           <t>30.00%</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="3" t="inlineStr">
         <is>
           <t>2025-04-17</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t>4进5</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" s="3" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E21" s="3" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" s="3" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="G21" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" t="n">
+      <c r="G21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="3" t="inlineStr">
         <is>
           <t>2025-04-17</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="inlineStr">
+      <c r="B22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
         <is>
           <t>5进6</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1</v>
-      </c>
-      <c r="I22" t="n">
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="3" t="inlineStr">
         <is>
           <t>2025-04-17</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="inlineStr">
+      <c r="B23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
         <is>
           <t>6进7</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" t="n">
+      <c r="G23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>2025-04-17</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" t="inlineStr">
+      <c r="B24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
         <is>
           <t>9进10</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" s="3" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" t="n">
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>2025-04-18</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>1进2</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr">
         <is>
           <t>23.68%</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E25" s="2" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" s="2" t="inlineStr">
         <is>
           <t>26.32%</t>
         </is>
       </c>
-      <c r="G25" t="n">
+      <c r="G25" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" s="2" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>2025-04-18</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>2进3</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E26" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="G26" t="n">
+      <c r="G26" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" s="2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>2025-04-18</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>3进4</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" s="2" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="G27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" t="n">
+      <c r="G27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>2025-04-18</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B28" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>4进5</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" s="2" t="inlineStr">
         <is>
           <t>40.00%</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E28" s="2" t="inlineStr">
         <is>
           <t>20.00%</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" s="2" t="inlineStr">
         <is>
           <t>40.00%</t>
         </is>
       </c>
-      <c r="G28" t="n">
+      <c r="G28" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="H28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I28" t="n">
+      <c r="H28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>2025-04-18</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" t="inlineStr">
+      <c r="B29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
         <is>
           <t>5进6</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" t="n">
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>2025-04-18</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="inlineStr">
+      <c r="B30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
         <is>
           <t>10进11</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
-        <v>1</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" t="n">
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B31" s="3" t="n">
         <v>68</v>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" s="3" t="inlineStr">
         <is>
           <t>1进2</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" s="3" t="inlineStr">
         <is>
           <t>16.18%</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E31" s="3" t="inlineStr">
         <is>
           <t>39.71%</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" s="3" t="inlineStr">
         <is>
           <t>44.12%</t>
         </is>
       </c>
-      <c r="G31" t="n">
+      <c r="G31" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" s="3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B32" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" s="3" t="inlineStr">
         <is>
           <t>2进3</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" s="3" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E32" s="3" t="inlineStr">
         <is>
           <t>20.00%</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" s="3" t="inlineStr">
         <is>
           <t>46.67%</t>
         </is>
       </c>
-      <c r="G32" t="n">
+      <c r="G32" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B33" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" s="3" t="inlineStr">
         <is>
           <t>3进4</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" s="3" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E33" s="3" t="inlineStr">
         <is>
           <t>25.00%</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" s="3" t="inlineStr">
         <is>
           <t>25.00%</t>
         </is>
       </c>
-      <c r="G33" t="n">
+      <c r="G33" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H33" t="n">
-        <v>1</v>
-      </c>
-      <c r="I33" t="n">
+      <c r="H33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B34" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" t="inlineStr">
+      <c r="B34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
         <is>
           <t>4进5</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" s="3" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G34" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" t="n">
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="B35" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C35" s="3" t="inlineStr">
         <is>
           <t>5进6</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" s="3" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E35" s="3" t="inlineStr">
         <is>
           <t>50.00%</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G35" t="n">
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G35" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H35" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I35" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="inlineStr">
+      <c r="B36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="inlineStr">
         <is>
           <t>6进7</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
+      <c r="D36" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E36" s="3" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" t="n">
-        <v>1</v>
-      </c>
-      <c r="I36" t="n">
+      <c r="F36" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" t="inlineStr">
+      <c r="B37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="inlineStr">
         <is>
           <t>8进9</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" s="3" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
+      <c r="E37" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F37" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="3" t="inlineStr">
         <is>
           <t>2025-04-21</t>
         </is>
       </c>
-      <c r="B38" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" t="inlineStr">
+      <c r="B38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="inlineStr">
         <is>
           <t>11进12</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" s="3" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B39" s="2" t="n">
         <v>51</v>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="C39" s="2" t="inlineStr">
         <is>
           <t>1进2</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" s="2" t="inlineStr">
         <is>
           <t>9.80%</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E39" s="2" t="inlineStr">
         <is>
           <t>27.45%</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" s="2" t="inlineStr">
         <is>
           <t>62.75%</t>
         </is>
       </c>
-      <c r="G39" t="n">
+      <c r="G39" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="H39" t="n">
+      <c r="H39" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39" s="2" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B40" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C40" s="2" t="inlineStr">
         <is>
           <t>2进3</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" s="2" t="inlineStr">
         <is>
           <t>27.27%</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E40" s="2" t="inlineStr">
         <is>
           <t>18.18%</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" s="2" t="inlineStr">
         <is>
           <t>54.55%</t>
         </is>
       </c>
-      <c r="G40" t="n">
+      <c r="G40" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="H40" t="n">
+      <c r="H40" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I40" s="2" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C41" s="2" t="inlineStr">
         <is>
           <t>3进4</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="2" t="inlineStr">
         <is>
           <t>40.00%</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
         <is>
           <t>60.00%</t>
         </is>
       </c>
-      <c r="G41" t="n">
+      <c r="G41" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
+      <c r="H41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="B42" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C42" s="2" t="inlineStr">
         <is>
           <t>4进5</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
         <is>
           <t>33.33%</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" s="2" t="inlineStr">
         <is>
           <t>66.67%</t>
         </is>
       </c>
-      <c r="G42" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>1</v>
-      </c>
-      <c r="I42" t="n">
+      <c r="G42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="B43" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C43" s="2" t="inlineStr">
         <is>
           <t>5进6</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G43" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" t="n">
+      <c r="G43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="B44" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="C44" s="2" t="inlineStr">
         <is>
           <t>6进7</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
+      <c r="G44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B45" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" t="inlineStr">
+      <c r="B45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="inlineStr">
         <is>
           <t>8进9</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="G45" t="n">
-        <v>1</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="n">
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B46" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" t="inlineStr">
+      <c r="B46" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
         <is>
           <t>9进10</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G46" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" t="n">
+      <c r="G46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="2" t="inlineStr">
         <is>
           <t>2025-04-22</t>
         </is>
       </c>
-      <c r="B47" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" t="inlineStr">
+      <c r="B47" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="inlineStr">
         <is>
           <t>12进13</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
       </c>
-      <c r="G47" t="n">
-        <v>0</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" t="n">
+      <c r="G47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily stock scores and save
</commit_message>
<xml_diff>
--- a/excel/limit_up_history.xlsx
+++ b/excel/limit_up_history.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="晋级率" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="每日热门" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -29,7 +30,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -46,6 +47,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00F2F2F2"/>
         <bgColor rgb="00F2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
+        <bgColor rgb="00D9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -67,13 +74,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -32098,4 +32108,3684 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="15" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>日期</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>股票代码</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>股票简称</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>几天几板</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>涨停原因类别</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>覆盖热点</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>热点数量</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>关注度排名</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>关注度加分</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>原始得分</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>总得分</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>600505.SH</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>西昌电力</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>电力+光伏发电+央企+扭亏为盈</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>['电力', '央企', '光伏']</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>2.684</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>4.667</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>7.351</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>600744.SH</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>华银电力</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>电力+一季报增长+光伏+国企</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>['一季报增长', '电力', '光伏']</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>2.263</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>7.263</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>002251.SZ</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>步步高</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>7天6板</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>零售+摘帽+一季报增长+年报扭亏</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>['一季报增长']</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>601956.SH</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>东贝集团</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>人形机器人+蜜雪冰城供应商+跨境电商</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>['人形机器人', '跨境电商']</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>2.833</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>3.833</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>003003.SZ</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>天元股份</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>6天6板</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>跨境电商+可降解塑料+快递包装</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>1.105</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>1.333</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>2.439</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>002648.SZ</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>卫星化学</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>一季报增长+此前股价受关税影响+化工+轻烃</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>['一季报增长']</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>000601.SZ</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>韶能股份</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>水电+分红回购+新能源车零部件</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>1.842</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>1.842</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>600051.SH</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>宁波联合</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>电力+房地产+进出口贸易</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>['电力']</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>1.833</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>1.833</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月25日</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>002095.SZ</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>生意宝</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>5天3板</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>跨境电商+数据要素</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1.333</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>002251.SZ</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>步步高</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>6天5板</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>零售+摘帽+一季报增长+年报扭亏</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>['一季报增长', '零售']</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>2.579</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>5.379</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>000965.SZ</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>天保基建</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>7天6板</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>房地产+大飞机+天津国企</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>['国企', '房地产']</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>1.947</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>4.547</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>600644.SH</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>乐山电力</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>9天7板</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>电力+光储</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>['电力']</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>2.368</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3" t="n">
+        <v>4.368</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>601086.SH</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>国芳集团</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>15天13板</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>地天板+零售+参股券商+参投御道智算</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>000632.SZ</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>三木集团</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>跨境电商+创投+福建国企</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>['跨境电商', '国企']</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>603696.SH</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>安记食品</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>8天7板</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>地天板+调味品+新零售+年报增长</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>1.842</v>
+      </c>
+      <c r="J16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3" t="n">
+        <v>2.842</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>002537.SZ</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>海联金汇</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>4天4板</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>跨境支付+汽车零部件</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>2.474</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <v>2.474</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>002427.SZ</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>尤夫股份</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>6天5板</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>拒海水聚酯工业丝+化纤+陕西国资+客户巨力索具</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>2.158</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3" t="n">
+        <v>2.158</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>603086.SH</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>先达股份</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>4天4板</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>一季报增长+烯草酮+农药+大豆</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>['一季报增长']</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>003003.SZ</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>天元股份</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>5天5板</t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>跨境电商+可降解塑料+快递包装</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K20" s="3" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>601956.SH</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>东贝集团</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>人形机器人+蜜雪冰城供应商+跨境电商</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K21" s="3" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>002693.SZ</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>双成药业</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>11天6板</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>资金博弈激烈+此前拟收购宁波奥拉半导体</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <v>1.421</v>
+      </c>
+      <c r="J22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3" t="n">
+        <v>1.421</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>002196.SZ</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>方正电机</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>机器人关节+新能源驱动电机+国企</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K23" s="3" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>002564.SZ</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>天沃科技</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>10天6板</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>摘帽+高端装备+业绩增长+上海国企改革</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K24" s="3" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月24日</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>002584.SZ</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>西陇科学</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>光刻胶+化学试剂+生物医药</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="I25" s="3" t="n">
+        <v>1.211</v>
+      </c>
+      <c r="J25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3" t="n">
+        <v>1.211</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>002537.SZ</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>海联金汇</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>跨境支付+汽车零部件</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>['汽车零部件', '跨境支付']</t>
+        </is>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>1.842</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>3.125</v>
+      </c>
+      <c r="K26" s="2" t="n">
+        <v>4.967</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>002251.SZ</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>步步高</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>5天4板</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>摘帽+零售+一季报增长+年报扭亏</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>['一季报增长']</t>
+        </is>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>2.895</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>1.375</v>
+      </c>
+      <c r="K27" s="2" t="n">
+        <v>4.27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>002094.SZ</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>青岛金王</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>跨境支付+中韩自贸区+蜡烛</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>['跨境支付']</t>
+        </is>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>2.684</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K28" s="2" t="n">
+        <v>4.184</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>601008.SH</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>连云港</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>14天9板</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>港口航运+国企</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>2.474</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>1.125</v>
+      </c>
+      <c r="K29" s="2" t="n">
+        <v>3.599</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>002427.SZ</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>尤夫股份</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>5天4板</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>拒海水聚酯工业丝+客户巨力索具+化纤+陕西国资</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>2.579</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="n">
+        <v>2.579</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>600790.SH</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>轻纺城</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>跨境电商+纺织面料+国企</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>['跨境电商', '国企']</t>
+        </is>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>000632.SZ</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>三木集团</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>跨境电商+创投+福建国企</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>['跨境电商', '国企']</t>
+        </is>
+      </c>
+      <c r="G32" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>600860.SH</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>京城股份</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>天工机器人夺冠+京城机电控股股东</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>['机器人']</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K33" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>603119.SH</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>浙江荣泰</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>机器人+战略布局未受关税实质影响+特斯拉供应链</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>['机器人']</t>
+        </is>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>002915.SZ</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>中欣氟材</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>业绩增长+PEEK材料+氟化工</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>['业绩增长']</t>
+        </is>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="K35" s="2" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>300542.SZ</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>新晨科技</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>拟收购天一恩华+跨境支付+华为</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>['跨境支付']</t>
+        </is>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
+          <t>603086.SH</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="inlineStr">
+        <is>
+          <t>先达股份</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>一季报增长+烯草酮+农药+大豆</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>['一季报增长']</t>
+        </is>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="2" t="n">
+        <v>1.375</v>
+      </c>
+      <c r="K37" s="2" t="n">
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月23日</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>003003.SZ</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>天元股份</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>4天4板</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>跨境电商+可降解塑料+快递包装</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="2" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="K38" s="2" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>603128.SH</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>华贸物流</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>6天4板</t>
+        </is>
+      </c>
+      <c r="E39" s="3" t="inlineStr">
+        <is>
+          <t>跨境电商+敦煌网合作+物流+国企改革</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>['跨境电商', '国企', '物流', '国企改革']</t>
+        </is>
+      </c>
+      <c r="G39" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="I39" s="3" t="n">
+        <v>1.105</v>
+      </c>
+      <c r="J39" s="3" t="n">
+        <v>6.571</v>
+      </c>
+      <c r="K39" s="3" t="n">
+        <v>7.677</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>600794.SH</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>保税科技</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>4天4板</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>智慧物流+数字货币+电子商务+国企</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>['国企', '物流', '电子商务']</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I40" s="3" t="n">
+        <v>2.263</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>4.857</v>
+      </c>
+      <c r="K40" s="3" t="n">
+        <v>7.12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>601086.SH</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>国芳集团</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>13天12板</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>零售+参股券商+参投御道智算+连续涨停+股价创历史新高</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" s="3" t="n">
+        <v>2.895</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>1.429</v>
+      </c>
+      <c r="K41" s="3" t="n">
+        <v>4.323</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>002094.SZ</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="inlineStr">
+        <is>
+          <t>青岛金王</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>年报净利增长+跨境支付+中韩自贸区+化妆品</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>['跨境支付']</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I42" s="3" t="n">
+        <v>2.579</v>
+      </c>
+      <c r="J42" s="3" t="n">
+        <v>1.571</v>
+      </c>
+      <c r="K42" s="3" t="n">
+        <v>4.15</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>000965.SZ</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="inlineStr">
+        <is>
+          <t>天保基建</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>5天5板</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="inlineStr">
+        <is>
+          <t>大飞机+房地产+天津国企</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="I43" s="3" t="n">
+        <v>1.842</v>
+      </c>
+      <c r="J43" s="3" t="n">
+        <v>1.857</v>
+      </c>
+      <c r="K43" s="3" t="n">
+        <v>3.699</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>002640.SZ</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>跨境通</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>跨境电商+欧美用户</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="I44" s="3" t="n">
+        <v>1.421</v>
+      </c>
+      <c r="J44" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K44" s="3" t="n">
+        <v>3.421</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>600571.SH</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="inlineStr">
+        <is>
+          <t>信雅达</t>
+        </is>
+      </c>
+      <c r="D45" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E45" s="3" t="inlineStr">
+        <is>
+          <t>跨境支付+金融科技+AI智能体+此前因Pika大涨</t>
+        </is>
+      </c>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>['跨境支付']</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I45" s="3" t="n">
+        <v>1.632</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <v>1.571</v>
+      </c>
+      <c r="K45" s="3" t="n">
+        <v>3.203</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>002165.SZ</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="inlineStr">
+        <is>
+          <t>红宝丽</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>6天5板</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>环氧丙烷衍生品+光刻胶+出海</t>
+        </is>
+      </c>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>603696.SH</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>安记食品</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="inlineStr">
+        <is>
+          <t>6天6板</t>
+        </is>
+      </c>
+      <c r="E47" s="3" t="inlineStr">
+        <is>
+          <t>调味品+新零售+年报增长</t>
+        </is>
+      </c>
+      <c r="F47" s="3" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="I47" s="3" t="n">
+        <v>1.526</v>
+      </c>
+      <c r="J47" s="3" t="n">
+        <v>1.429</v>
+      </c>
+      <c r="K47" s="3" t="n">
+        <v>2.955</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>002537.SZ</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>海联金汇</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>跨境支付+汽车零部件</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="inlineStr">
+        <is>
+          <t>['跨境支付']</t>
+        </is>
+      </c>
+      <c r="G48" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="I48" s="3" t="n">
+        <v>1.211</v>
+      </c>
+      <c r="J48" s="3" t="n">
+        <v>1.571</v>
+      </c>
+      <c r="K48" s="3" t="n">
+        <v>2.782</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>002251.SZ</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="inlineStr">
+        <is>
+          <t>步步高</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="inlineStr">
+        <is>
+          <t>4天3板</t>
+        </is>
+      </c>
+      <c r="E49" s="3" t="inlineStr">
+        <is>
+          <t>摘帽+零售+一季报增长+年报扭亏</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G49" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I49" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" s="3" t="n">
+        <v>1.429</v>
+      </c>
+      <c r="K49" s="3" t="n">
+        <v>2.429</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t>600644.SH</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="inlineStr">
+        <is>
+          <t>乐山电力</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>7天6板</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>电力+光储</t>
+        </is>
+      </c>
+      <c r="F50" s="3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="I50" s="3" t="n">
+        <v>2.368</v>
+      </c>
+      <c r="J50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3" t="n">
+        <v>2.368</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>003003.SZ</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="inlineStr">
+        <is>
+          <t>天元股份</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E51" s="3" t="inlineStr">
+        <is>
+          <t>跨境电商+可降解塑料+快递包装</t>
+        </is>
+      </c>
+      <c r="F51" s="3" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G51" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K51" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B52" s="3" t="inlineStr">
+        <is>
+          <t>002095.SZ</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>生意宝</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>跨境电商+数据要素</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G52" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K52" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>601008.SH</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>连云港</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>13天8板</t>
+        </is>
+      </c>
+      <c r="E53" s="3" t="inlineStr">
+        <is>
+          <t>港口航运+国企</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3" t="n">
+        <v>1.857</v>
+      </c>
+      <c r="K53" s="3" t="n">
+        <v>1.857</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B54" s="3" t="inlineStr">
+        <is>
+          <t>002564.SZ</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="inlineStr">
+        <is>
+          <t>天沃科技</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>8天5板</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>摘帽+电力设计+高端装备+上海国企</t>
+        </is>
+      </c>
+      <c r="F54" s="3" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G54" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" s="3" t="n">
+        <v>1.857</v>
+      </c>
+      <c r="K54" s="3" t="n">
+        <v>1.857</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>600865.SH</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="inlineStr">
+        <is>
+          <t>百大集团</t>
+        </is>
+      </c>
+      <c r="D55" s="3" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E55" s="3" t="inlineStr">
+        <is>
+          <t>年报净利增长+零售+杭州</t>
+        </is>
+      </c>
+      <c r="F55" s="3" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G55" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3" t="n">
+        <v>1.429</v>
+      </c>
+      <c r="K55" s="3" t="n">
+        <v>1.429</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B56" s="3" t="inlineStr">
+        <is>
+          <t>603697.SH</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="inlineStr">
+        <is>
+          <t>有友食品</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr">
+        <is>
+          <t>泡凤爪+新零售+年报增长</t>
+        </is>
+      </c>
+      <c r="F56" s="3" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G56" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>1.429</v>
+      </c>
+      <c r="K56" s="3" t="n">
+        <v>1.429</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B57" s="3" t="inlineStr">
+        <is>
+          <t>603839.SH</t>
+        </is>
+      </c>
+      <c r="C57" s="3" t="inlineStr">
+        <is>
+          <t>安正时尚</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E57" s="3" t="inlineStr">
+        <is>
+          <t>服装+电子商务</t>
+        </is>
+      </c>
+      <c r="F57" s="3" t="inlineStr">
+        <is>
+          <t>['电子商务']</t>
+        </is>
+      </c>
+      <c r="G57" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>1.286</v>
+      </c>
+      <c r="K57" s="3" t="n">
+        <v>1.286</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="inlineStr">
+        <is>
+          <t>2025年04月22日</t>
+        </is>
+      </c>
+      <c r="B58" s="3" t="inlineStr">
+        <is>
+          <t>603351.SH</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="inlineStr">
+        <is>
+          <t>威尔药业</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>业绩增长+药用辅料+润滑油+国际贸易影响小</t>
+        </is>
+      </c>
+      <c r="F58" s="3" t="inlineStr">
+        <is>
+          <t>['业绩增长']</t>
+        </is>
+      </c>
+      <c r="G58" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>1.143</v>
+      </c>
+      <c r="K58" s="3" t="n">
+        <v>1.143</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>601086.SH</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="inlineStr">
+        <is>
+          <t>国芳集团</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>12天11板</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>零售+参股券商+参投御道智算</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G59" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I59" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K59" s="2" t="n">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>000965.SZ</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>天保基建</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>4天4板</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>房地产+大飞机+天津国企</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>['国企', '大飞机']</t>
+        </is>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="I60" s="2" t="n">
+        <v>1.105</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K60" s="2" t="n">
+        <v>4.105</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>600794.SH</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="inlineStr">
+        <is>
+          <t>保税科技</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>智慧物流+数字货币+电子商务+国企</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="I61" s="2" t="n">
+        <v>2.263</v>
+      </c>
+      <c r="J61" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K61" s="2" t="n">
+        <v>4.063</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>002251.SZ</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>步步高</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>摘帽+零售+胖东来帮扶+年报扭亏</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I62" s="2" t="n">
+        <v>2.158</v>
+      </c>
+      <c r="J62" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K62" s="2" t="n">
+        <v>3.558</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="inlineStr">
+        <is>
+          <t>000859.SZ</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="inlineStr">
+        <is>
+          <t>国风新材</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>光刻胶+集成电路PI材料+聚丙烯薄膜+国企</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>['国企']</t>
+        </is>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="I63" s="2" t="n">
+        <v>1.211</v>
+      </c>
+      <c r="J63" s="2" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K63" s="2" t="n">
+        <v>3.011</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>600865.SH</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>百大集团</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>年报净利增长+零售+杭州</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>['年报净利增长', '零售']</t>
+        </is>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H64" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="K64" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B65" s="2" t="inlineStr">
+        <is>
+          <t>605188.SH</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="inlineStr">
+        <is>
+          <t>国光连锁</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>6天6板</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>零售+生鲜食品+智能物流</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="I65" s="2" t="n">
+        <v>1.526</v>
+      </c>
+      <c r="J65" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K65" s="2" t="n">
+        <v>2.926</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>002583.SZ</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>海能达</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>6G+对讲机终端+一带一路</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I66" s="2" t="n">
+        <v>2.895</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="2" t="n">
+        <v>2.895</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B67" s="2" t="inlineStr">
+        <is>
+          <t>600644.SH</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="inlineStr">
+        <is>
+          <t>乐山电力</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>6天5板</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>电力+光储</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I67" s="2" t="n">
+        <v>2.579</v>
+      </c>
+      <c r="J67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" s="2" t="n">
+        <v>2.579</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>003003.SZ</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>天元股份</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>跨境电商+可降解塑料+快递包装</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>['跨境电商']</t>
+        </is>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K68" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
+        <is>
+          <t>600391.SH</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="inlineStr">
+        <is>
+          <t>航发科技</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>航空发动机+军工+央企+年报净利增长</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>['年报净利增长']</t>
+        </is>
+      </c>
+      <c r="G69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K69" s="2" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>603042.SH</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>华脉科技</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>2天2板</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>年报净利增长+铜缆高速连接+数据中心+通信设备</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>['年报净利增长']</t>
+        </is>
+      </c>
+      <c r="G70" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="K70" s="2" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>002153.SZ</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="inlineStr">
+        <is>
+          <t>石基信息</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>跨境支付+大消费行业信息管理软件+云酒店信息系统+阿里合作</t>
+        </is>
+      </c>
+      <c r="F71" s="2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="I71" s="2" t="n">
+        <v>1.421</v>
+      </c>
+      <c r="J71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" s="2" t="n">
+        <v>1.421</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>603237.SH</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>五芳斋</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr">
+        <is>
+          <t>食品加工制造+新零售+市场拓展</t>
+        </is>
+      </c>
+      <c r="F72" s="2" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K72" s="2" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B73" s="2" t="inlineStr">
+        <is>
+          <t>603696.SH</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="inlineStr">
+        <is>
+          <t>安记食品</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>5天5板</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="inlineStr">
+        <is>
+          <t>调味品+新零售</t>
+        </is>
+      </c>
+      <c r="F73" s="2" t="inlineStr">
+        <is>
+          <t>['零售']</t>
+        </is>
+      </c>
+      <c r="G73" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K73" s="2" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>002427.SZ</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>尤夫股份</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>3天3板</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="inlineStr">
+        <is>
+          <t>拒海水聚酯工业丝+客户巨力索具+化纤+陕西国资</t>
+        </is>
+      </c>
+      <c r="F74" s="2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="G74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="I74" s="2" t="n">
+        <v>1.316</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" s="2" t="n">
+        <v>1.316</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B75" s="2" t="inlineStr">
+        <is>
+          <t>001316.SZ</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="inlineStr">
+        <is>
+          <t>润贝航科</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="inlineStr">
+        <is>
+          <t>大飞机+航空材料+AI眼镜+低空经济</t>
+        </is>
+      </c>
+      <c r="F75" s="2" t="inlineStr">
+        <is>
+          <t>['大飞机']</t>
+        </is>
+      </c>
+      <c r="G75" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K75" s="2" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>2025年04月21日</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
+        <is>
+          <t>603900.SH</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
+          <t>莱绅通灵</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>3天2板</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="inlineStr">
+        <is>
+          <t>黄金+珠宝首饰+IP</t>
+        </is>
+      </c>
+      <c r="F76" s="2" t="inlineStr">
+        <is>
+          <t>['黄金']</t>
+        </is>
+      </c>
+      <c r="G76" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" s="2" t="inlineStr">
+        <is>
+          <t>未上榜</t>
+        </is>
+      </c>
+      <c r="I76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K76" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
little improve and data update
</commit_message>
<xml_diff>
--- a/excel/limit_up_history.xlsx
+++ b/excel/limit_up_history.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P540"/>
+  <dimension ref="A1:P547"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36122,6 +36122,468 @@
         <v>0</v>
       </c>
     </row>
+    <row r="541">
+      <c r="A541" s="3" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="B541" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="C541" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="D541" s="3" t="inlineStr">
+        <is>
+          <t>1进2</t>
+        </is>
+      </c>
+      <c r="E541" s="3" t="inlineStr">
+        <is>
+          <t>26.92%</t>
+        </is>
+      </c>
+      <c r="F541" s="3" t="inlineStr">
+        <is>
+          <t>61.54%</t>
+        </is>
+      </c>
+      <c r="G541" s="3" t="inlineStr">
+        <is>
+          <t>38.46%</t>
+        </is>
+      </c>
+      <c r="H541" s="3" t="inlineStr">
+        <is>
+          <t>38.89%</t>
+        </is>
+      </c>
+      <c r="I541" s="3" t="inlineStr">
+        <is>
+          <t>83.33%</t>
+        </is>
+      </c>
+      <c r="J541" s="3" t="inlineStr">
+        <is>
+          <t>16.67%</t>
+        </is>
+      </c>
+      <c r="K541" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="L541" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="M541" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="N541" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="O541" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="P541" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="3" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="B542" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="C542" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D542" s="3" t="inlineStr">
+        <is>
+          <t>2进3</t>
+        </is>
+      </c>
+      <c r="E542" s="3" t="inlineStr">
+        <is>
+          <t>11.11%</t>
+        </is>
+      </c>
+      <c r="F542" s="3" t="inlineStr">
+        <is>
+          <t>55.56%</t>
+        </is>
+      </c>
+      <c r="G542" s="3" t="inlineStr">
+        <is>
+          <t>44.44%</t>
+        </is>
+      </c>
+      <c r="H542" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="I542" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="J542" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="K542" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L542" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M542" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="N542" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O542" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P542" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="3" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="B543" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C543" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D543" s="3" t="inlineStr">
+        <is>
+          <t>3进4</t>
+        </is>
+      </c>
+      <c r="E543" s="3" t="inlineStr">
+        <is>
+          <t>71.43%</t>
+        </is>
+      </c>
+      <c r="F543" s="3" t="inlineStr">
+        <is>
+          <t>71.43%</t>
+        </is>
+      </c>
+      <c r="G543" s="3" t="inlineStr">
+        <is>
+          <t>28.57%</t>
+        </is>
+      </c>
+      <c r="H543" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="I543" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="J543" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="K543" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L543" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M543" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N543" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="O543" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="P543" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="3" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="B544" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C544" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D544" s="3" t="inlineStr">
+        <is>
+          <t>4进5</t>
+        </is>
+      </c>
+      <c r="E544" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F544" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G544" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="H544" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="I544" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="J544" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="K544" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L544" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M544" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N544" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O544" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P544" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="3" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="B545" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C545" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D545" s="3" t="inlineStr">
+        <is>
+          <t>5进6</t>
+        </is>
+      </c>
+      <c r="E545" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="F545" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="G545" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="H545" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="I545" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="J545" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="K545" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L545" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M545" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N545" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O545" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P545" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="3" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="B546" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C546" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D546" s="3" t="inlineStr">
+        <is>
+          <t>7进8</t>
+        </is>
+      </c>
+      <c r="E546" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="F546" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="G546" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="H546" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="I546" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="J546" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="K546" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L546" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M546" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N546" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O546" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P546" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="3" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="B547" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C547" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D547" s="3" t="inlineStr">
+        <is>
+          <t>8进9</t>
+        </is>
+      </c>
+      <c r="E547" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="F547" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="G547" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="H547" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="I547" s="3" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="J547" s="3" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="K547" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L547" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M547" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N547" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O547" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P547" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>